<commit_message>
Merise emp Analyse #1
</commit_message>
<xml_diff>
--- a/merise/intro_gestion_employes/Merise - intro - gestion employes.xlsx
+++ b/merise/intro_gestion_employes/Merise - intro - gestion employes.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MDevoldere\github\DWWM_2005\merise\intro_gestion_employes\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57465324-D056-44C5-920C-24FFF089799A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -18,9 +24,50 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="12">
+  <si>
+    <t>co_name</t>
+  </si>
+  <si>
+    <t>co_siren</t>
+  </si>
+  <si>
+    <t>emp_name</t>
+  </si>
+  <si>
+    <t>emp_id</t>
+  </si>
+  <si>
+    <t>emp_email</t>
+  </si>
+  <si>
+    <t>emp_role</t>
+  </si>
+  <si>
+    <t>emp_firstname</t>
+  </si>
+  <si>
+    <t>dept_name</t>
+  </si>
+  <si>
+    <t>dept_building</t>
+  </si>
+  <si>
+    <t>dept_floor</t>
+  </si>
+  <si>
+    <t>Matrice des dépendances fonctionnelles</t>
+  </si>
+  <si>
+    <t>Simplication (supression des colonnes sans "1")</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -28,16 +75,46 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -45,12 +122,169 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +564,334 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Q13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N19" sqref="N18:N19"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A1" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N3" s="3"/>
+      <c r="O3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="P3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q3" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9">
+        <v>1</v>
+      </c>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="N4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="O4" s="9"/>
+      <c r="P4" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="10"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="9">
+        <v>1</v>
+      </c>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9">
+        <v>1</v>
+      </c>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="N5" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="O5" s="9">
+        <v>1</v>
+      </c>
+      <c r="P5" s="9"/>
+      <c r="Q5" s="10"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="N6" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="O6" s="9"/>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="10"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9">
+        <v>1</v>
+      </c>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="N7" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="O7" s="9"/>
+      <c r="P7" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="10"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9">
+        <v>1</v>
+      </c>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="N8" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="O8" s="9"/>
+      <c r="P8" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="10"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9">
+        <v>1</v>
+      </c>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="N9" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="O9" s="9"/>
+      <c r="P9" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="10"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9">
+        <v>1</v>
+      </c>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="N10" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="O10" s="9"/>
+      <c r="P10" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="10"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9">
+        <v>1</v>
+      </c>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="N11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="O11" s="9"/>
+      <c r="P11" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="10"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9">
+        <v>1</v>
+      </c>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9">
+        <v>1</v>
+      </c>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="N12" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="O12" s="9"/>
+      <c r="P12" s="9"/>
+      <c r="Q12" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9">
+        <v>1</v>
+      </c>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9">
+        <v>1</v>
+      </c>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="N13" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="O13" s="11"/>
+      <c r="P13" s="11"/>
+      <c r="Q13" s="12">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>